<commit_message>
rebased replacement levels, added new features to shiny app
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0C5623-0108-4548-8E12-7D118E34DBAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1DA24-6391-4C4E-9C4C-B2EA9D048F63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6660" yWindow="4824" windowWidth="14172" windowHeight="11052" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8594" uniqueCount="7850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8639" uniqueCount="7851">
   <si>
     <t>drafted</t>
   </si>
@@ -23549,9 +23549,6 @@
     <t>ds9</t>
   </si>
   <si>
-    <t>drjames</t>
-  </si>
-  <si>
     <t>DH</t>
   </si>
   <si>
@@ -23577,6 +23574,12 @@
   </si>
   <si>
     <t>Spencer Torkelson</t>
+  </si>
+  <si>
+    <t>Jasson Dominguez</t>
+  </si>
+  <si>
+    <t>lacugna</t>
   </si>
 </sst>
 </file>
@@ -23586,13 +23589,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0;[Red]\$#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF3E3F40"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -23615,13 +23624,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23903,10 +23913,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E474"/>
+  <dimension ref="A1:F373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G219" sqref="G219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23916,21 +23926,21 @@
     <col min="3" max="3" width="8.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.88671875" customWidth="1"/>
+    <col min="6" max="1024" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7841</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7842</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7843</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>7844</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7845</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -23940,7 +23950,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2">
@@ -23957,7 +23967,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>502</v>
       </c>
       <c r="C3" s="2">
@@ -23974,7 +23984,7 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>473</v>
       </c>
       <c r="C4" s="2">
@@ -23991,7 +24001,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>387</v>
       </c>
       <c r="C5" s="2">
@@ -24008,7 +24018,7 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>432</v>
       </c>
       <c r="C6" s="2">
@@ -24025,7 +24035,7 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2">
@@ -24042,7 +24052,7 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>319</v>
       </c>
       <c r="C8" s="2">
@@ -24059,7 +24069,7 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C9" s="2">
@@ -24076,7 +24086,7 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>618</v>
       </c>
       <c r="C10" s="2">
@@ -24093,14 +24103,14 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>7841</v>
+        <v>7840</v>
       </c>
       <c r="E11" s="3">
         <v>44192</v>
@@ -24110,8 +24120,8 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>7847</v>
+      <c r="B12" s="1" t="s">
+        <v>7846</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -24127,7 +24137,7 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>1965</v>
       </c>
       <c r="C13" s="2">
@@ -24213,7 +24223,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7848</v>
+        <v>7847</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -24338,7 +24348,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>7841</v>
+        <v>7840</v>
       </c>
       <c r="E25" s="3">
         <v>44192</v>
@@ -24944,7 +24954,7 @@
         <v>92</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>7846</v>
+        <v>7845</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
@@ -24967,7 +24977,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>7831</v>
       </c>
       <c r="E62" s="3">
         <v>44192</v>
@@ -25182,7 +25192,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>7849</v>
+        <v>7848</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -25324,7 +25334,7 @@
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>7841</v>
+        <v>7840</v>
       </c>
       <c r="E83" s="3">
         <v>44192</v>
@@ -25332,7 +25342,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>454</v>
@@ -25349,7 +25359,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>116</v>
@@ -25366,7 +25376,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>105</v>
@@ -25383,7 +25393,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>110</v>
@@ -25400,7 +25410,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>106</v>
@@ -25417,7 +25427,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>112</v>
@@ -25434,7 +25444,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>113</v>
@@ -25451,7 +25461,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>503</v>
@@ -25468,7 +25478,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>7840</v>
+        <v>7850</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>108</v>
@@ -25834,7 +25844,7 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>7841</v>
+        <v>7840</v>
       </c>
       <c r="E113" s="3">
         <v>44192</v>
@@ -26881,7 +26891,7 @@
       <c r="A175" t="s">
         <v>178</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="1" t="s">
         <v>397</v>
       </c>
       <c r="C175" s="2">
@@ -27000,7 +27010,7 @@
       <c r="A182" t="s">
         <v>178</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>188</v>
       </c>
       <c r="C182" s="2">
@@ -27183,7 +27193,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>190</v>
       </c>
@@ -27200,7 +27210,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>190</v>
       </c>
@@ -27217,7 +27227,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>203</v>
       </c>
@@ -27234,7 +27244,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>203</v>
       </c>
@@ -27251,7 +27261,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>203</v>
       </c>
@@ -27268,7 +27278,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>203</v>
       </c>
@@ -27285,7 +27295,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>203</v>
       </c>
@@ -27302,7 +27312,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>203</v>
       </c>
@@ -27319,7 +27329,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>203</v>
       </c>
@@ -27336,7 +27346,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -27353,7 +27363,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>203</v>
       </c>
@@ -27370,7 +27380,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -27387,7 +27397,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -27404,7 +27414,7 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>203</v>
       </c>
@@ -27421,15 +27431,279 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="224" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" spans="4:4" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D272" s="2"/>
-    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>79</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C207" s="2">
+        <v>12</v>
+      </c>
+      <c r="D207" t="s">
+        <v>7831</v>
+      </c>
+      <c r="E207" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F207" s="4"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>117</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C208" s="2">
+        <v>2</v>
+      </c>
+      <c r="D208" t="s">
+        <v>12</v>
+      </c>
+      <c r="E208" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F208" s="4"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>7850</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C209" s="2">
+        <v>4</v>
+      </c>
+      <c r="D209" t="s">
+        <v>12</v>
+      </c>
+      <c r="E209" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F209" s="4"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>7850</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C210" s="2">
+        <v>5</v>
+      </c>
+      <c r="D210" t="s">
+        <v>12</v>
+      </c>
+      <c r="E210" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F210" s="4"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>141</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C211" s="2">
+        <v>3</v>
+      </c>
+      <c r="D211" t="s">
+        <v>12</v>
+      </c>
+      <c r="E211" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F211" s="4"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>54</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C212" s="2">
+        <v>19</v>
+      </c>
+      <c r="D212" t="s">
+        <v>81</v>
+      </c>
+      <c r="E212" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F212" s="4"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>154</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>7849</v>
+      </c>
+      <c r="C213" s="2">
+        <v>0</v>
+      </c>
+      <c r="D213" t="s">
+        <v>26</v>
+      </c>
+      <c r="E213" s="3">
+        <v>44196</v>
+      </c>
+      <c r="F213" s="4"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>7838</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C214" s="2">
+        <v>26</v>
+      </c>
+      <c r="D214" t="s">
+        <v>7</v>
+      </c>
+      <c r="E214" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F214" s="4"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>1</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C215" s="2">
+        <v>44</v>
+      </c>
+      <c r="D215" t="s">
+        <v>81</v>
+      </c>
+      <c r="E215" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F215" s="4"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>7839</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C216" s="2">
+        <v>16</v>
+      </c>
+      <c r="D216" t="s">
+        <v>12</v>
+      </c>
+      <c r="E216" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F216" s="4"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>190</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C217" s="2">
+        <v>28</v>
+      </c>
+      <c r="D217" t="s">
+        <v>7</v>
+      </c>
+      <c r="E217" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F217" s="4"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>203</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C218" s="2">
+        <v>15</v>
+      </c>
+      <c r="D218" t="s">
+        <v>7830</v>
+      </c>
+      <c r="E218" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F218" s="4"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>7850</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C219" s="2">
+        <v>47</v>
+      </c>
+      <c r="D219" t="s">
+        <v>7830</v>
+      </c>
+      <c r="E219" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F219" s="4"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>141</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C220" s="2">
+        <v>18</v>
+      </c>
+      <c r="D220" t="s">
+        <v>7</v>
+      </c>
+      <c r="E220" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F220" s="4"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>117</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C221" s="2">
+        <v>42</v>
+      </c>
+      <c r="D221" t="s">
+        <v>12</v>
+      </c>
+      <c r="E221" s="3">
+        <v>44208</v>
+      </c>
+      <c r="F221" s="4"/>
+    </row>
+    <row r="224" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A474" s="2"/>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E474">
     <sortCondition ref="A2:A474"/>

</xml_diff>